<commit_message>
finales Review von Sven
</commit_message>
<xml_diff>
--- a/Review_Sven.xlsx
+++ b/Review_Sven.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="251">
   <si>
     <t>Title</t>
   </si>
@@ -706,6 +707,202 @@
   </si>
   <si>
     <t>7</t>
+  </si>
+  <si>
+    <t>keine AR-Benfiits, nur Bezug auf die wissenschaftl. Agrumentation</t>
+  </si>
+  <si>
+    <t>2,6,22</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>The face-to-face setting allows for traditional
+pedagogic communication.</t>
+  </si>
+  <si>
+    <t>To summarize all ratings above 2,00 (highest grades) the
+majority of students think: Construct3D is “easy to use”, “offers
+all functions to solve tasks efficiently”, “uses comprehensible
+terms in menus”, “offers good opportunities to stop the task and
+continue at the same point later on”, “allows to change easily
+between menus”, “can be used in a consistent way” (highest
+overall grade!), “requires in case of errors low effort to correct
+them”, “requires little time to learn”, “encourages to try new
+functions”, “does not require the user to remember many details”
+and “is designed in a way that things you learned once are
+memorized well”.</t>
+  </si>
+  <si>
+    <t>trotzdem gut geeigente da auf benefits von AR-ausgerichtet</t>
+  </si>
+  <si>
+    <t>The categories “self-descriptiveness” and “conformity with user
+expectations” got lower grades than the rest.</t>
+  </si>
+  <si>
+    <t>durch selbst-erklärenden Umgang und intuitive bedienbarkeit, schneller Umgang um das System für das Lernen zu verwenden. (Im Ggs. Zu herkömmlichen methoden?)</t>
+  </si>
+  <si>
+    <t>durch HDM-AR ist trotz dem Fokus auf das lernmaterial eine Face-to-Face situation möglich</t>
+  </si>
+  <si>
+    <t>The main advantage of using AR is that students actually see three
+dimensional objects which they until now had to calculate and
+construct with traditional - mostly pen and paper - methods
+(Figure 1 middle).</t>
+  </si>
+  <si>
+    <t>3D Modellierung ermöglichst bessere Vorstellbarkeit im ggs. Zu 2D pen and paper methoden</t>
+  </si>
+  <si>
+    <t>The learning performance of the AR-guided group was thus superior to
+that of the other two groups.</t>
+  </si>
+  <si>
+    <t>Multiple-comparisons analysis (LSD)
+revealed that the antecedents of flow did not differ significantly between the nonguided and audio-guided groups (p ¼ 0.297 &gt; 0.05), but
+was significantly higher for the AR-guided group than for both the nonguided (p ¼ 0.001 &lt;0.01) and audio-guided (p ¼ 0.012 &lt; 0.05) groups.</t>
+  </si>
+  <si>
+    <t>Post-hoc comparisons showed that the time spent focusing on paintings was significantly
+longer for both the AR-guided (mean ¼ 17.3278 min) and audio-guided (mean ¼ 16.114 min) groups than for the nonguided group
+(mean ¼ 4.76 min). The focusing time did not differ significantly between the AR-guided and audio-guided groups.</t>
+  </si>
+  <si>
+    <t>andere handlungsabfolgen und dadurch intensivere auseinander setzung mit dem "lernstoff" dadurch größerer lerneffekt, auch einbindung von virtuellen infos in reale welt</t>
+  </si>
+  <si>
+    <t>It facilitates the development of art appreciation by imprinting the knowledge of paintings on visitors’ memories, supporting
+the coupling between the visitors, the guide system, and the artwork (Klopfer &amp; Squire, 2008) by using AR technology, and helping visitors keep their memories of the artwork vivid. This also shows the necessity of the HCCI (Sung, Chang, et al., 2010).</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>9-10</t>
+  </si>
+  <si>
+    <t>Analysis of the flow experience revealed that the visitors in the AR-guided group were clearly more ready to enter the state of flow with
+respect to the antecedents of flow, and were more proactive in appreciating the artwork than were those in the other two groups. During the
+activity, those in the audio-guided and AR-guided groups expressed the flow states obviously.</t>
+  </si>
+  <si>
+    <t>more proactivity in appreciating the artwork</t>
+  </si>
+  <si>
+    <t>Observation/ Lernen von Mond und Sonnenphasen ohne Restriction durch natürliche Witterungsbedingungen u.Ä.</t>
+  </si>
+  <si>
+    <t>1,10</t>
+  </si>
+  <si>
+    <t>3-4</t>
+  </si>
+  <si>
+    <t>Overall, student responses to affective items showed a positive shift in their attitudes about their ability to understand focal topics and do
+science related skills. The mean affective score increased by 0.26 points (pre_mean ¼ 3.88   0.5, post_mean ¼ 4.14   0.58), with a moderate
+effect size of 0.48, meaning that the average increase in student scores was about one half of a standard deviation.</t>
+  </si>
+  <si>
+    <t>We witnessed significant learning gains on the content survey (T(70,1) ¼  8.53, based on paired t-test). Students’ scores went up by an
+average of 19% from the pre to post survey (Mean_pre ¼ 4.3   1.8, Mean_post ¼ 5.9   1.9, based on 9 total points). The effect size associated
+with these gains was substantial (1.0), indicating that student gains were equivalent to one standard deviation around the mean of the data.</t>
+  </si>
+  <si>
+    <t>Prior to the field trip, two of the teachers had expressed concern that the smartphones might be too engaging; leading students to ignore
+the real environment in favor of the media and capabilities provided by the smartphones. Post-field trip comments indicated the contrary
+was true – teachers noted that the smartphones promoted interaction with the pond and classmates.</t>
+  </si>
+  <si>
+    <t>Teachers commented that the smartphones helped to structure students’ movement through space and guided their interaction with the
+pond and with classmates. The students were able to work independently, at their own pace, with the teacher acting as a facilitator. Teachers
+reported that the activities were more student-driven and less teacher-directed.</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Another feature of the activity was the opportunity for collaborative communication and problem-solving among students that arose
+from the augmented reality experience.</t>
+  </si>
+  <si>
+    <t>Written feedback from the teachers indicated that AR was particularly useful in engaging students.</t>
+  </si>
+  <si>
+    <t>9-11</t>
+  </si>
+  <si>
+    <t>Guter Artikel!</t>
+  </si>
+  <si>
+    <t>The experimental group experienced higher levels of concentration on tasks
+(M ¼ 4.02, SD ¼ 0.60) than the control group (M ¼ 3.49, SD ¼ 0.83) [t ¼ 2.771, df ¼ 58, p-value ¼ 0.008, d ¼ 0.87]. Furthermore, AR-based
+application users had a higher sense of control (M ¼ 3.79, SD ¼ 0.53) than web-based application users (M ¼ 3.42, SD ¼ 0.59) [t ¼  2.505,
+df ¼ 57.923, p-value ¼ 0.015, d ¼ 0.68]. Finally, the experimental group reported a higher distorted sense of time (M ¼ 3.37, SD ¼ 0.92) than the control group (M ¼ 2.85, SD ¼ 0.71) [t ¼  2.392, df ¼ 50.366, p-value ¼ 0.02, d ¼ 0.56] (see Fig. 5).</t>
+  </si>
+  <si>
+    <t>Results indicate
+that the experimental group had higher levels of clear and direct feedback factor (M ¼ 3.64, SD ¼ 0.48) than the control group (M ¼ 3.27,
+SD ¼ 0.64) [U ¼ 303.5, p-value ¼ 0.03, d ¼ 0.58]. Similarly, the experimental group had higher values of autotelic experience (M ¼ 4.20,
+SD ¼ 0.71) than the control group (M¼ 3.63, SD ¼ 0.69) [U ¼ 243.5, p-value ¼ 0.002, d ¼ 0.86] (see Fig. 6).</t>
+  </si>
+  <si>
+    <t>Results showed that students were less bored and more in flow state
+when the AR-based application was used during the Magnet_2 stage.</t>
+  </si>
+  <si>
+    <t>Results showed that there are differences in students’ learning outcomes depending on which of the two learning applications they used.
+Indeed, students using the AR-based application performed significantly higher in the posttest than those that had used the web-based
+application.</t>
+  </si>
+  <si>
+    <t>Guter Artikel! Zusammenfassende ergebnisse auf Seite 11-12 besser zu verwenden</t>
+  </si>
+  <si>
+    <t>Gaming/Discovery</t>
+  </si>
+  <si>
+    <t>One of the advantages of an AR book over traditional book is that...</t>
+  </si>
+  <si>
+    <t>7-8</t>
+  </si>
+  <si>
+    <t>Nein/Ja?</t>
+  </si>
+  <si>
+    <t>eher nein, da der vergleich nur in einem Satz gezogen wird und nicht auf Empirie beruht. Die Vorteile sind nur in zwei sätzen aufgezeigt, wie bereits in allen anderen Artikeln auch bereits gefunden (Interesse/Engagement)</t>
+  </si>
+  <si>
+    <t>6-7</t>
+  </si>
+  <si>
+    <t>keine Benefits</t>
+  </si>
+  <si>
+    <t>Skills/Discovery</t>
+  </si>
+  <si>
+    <t>The analysis indicated that the participants with the ARsupported
+simulation gave significantly higher ratings in
+perceived skill development than those in the non-ARsupported
+groups.</t>
+  </si>
+  <si>
+    <t>Individual post-test results showed that participants in the
+AR-supported groups got significantly higher scores than
+those in the non-AR-supported groups (See Table II).</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>11-14</t>
+  </si>
+  <si>
+    <t>only significant benefit in 5.2.2, ansonsten keine Vorteile ggü. conventional library instructions</t>
   </si>
 </sst>
 </file>
@@ -1081,16 +1278,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M65"/>
+  <dimension ref="A1:M85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M62" sqref="M62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
     <col min="6" max="6" width="19.28515625" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
@@ -1289,7 +1486,7 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1390,6 +1587,9 @@
       <c r="L8" s="2" t="s">
         <v>159</v>
       </c>
+      <c r="M8" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -1500,7 +1700,7 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1535,7 +1735,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
+      <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -1586,6 +1786,9 @@
       </c>
       <c r="L14" s="2" t="s">
         <v>159</v>
+      </c>
+      <c r="M14" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1664,7 +1867,7 @@
       <c r="A19">
         <v>13</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -2003,6 +2206,18 @@
       <c r="G29" s="2" t="s">
         <v>140</v>
       </c>
+      <c r="H29" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J29" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="L29" t="s">
+        <v>158</v>
+      </c>
+      <c r="M29" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
@@ -2026,111 +2241,108 @@
       <c r="G30" s="2" t="s">
         <v>138</v>
       </c>
+      <c r="H30" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="J30" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="L30" t="s">
+        <v>158</v>
+      </c>
+      <c r="M30" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="I31" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="J31" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="K31" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="I32" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="J32" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="I33" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="J33" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="K33" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>24</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B34" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="G31" s="2" t="s">
+      <c r="E34" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G34" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>25</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>26</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>27</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>28</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>145</v>
@@ -2141,154 +2353,144 @@
       <c r="G35" s="2" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>29</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D36" s="2" t="s">
+      <c r="H35" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="J35" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="L35" t="s">
+        <v>159</v>
+      </c>
+      <c r="M35" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="J36" s="9" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="J37" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="J38" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="K38" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="J39" s="9" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="J40" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="K40" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>26</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="G36" s="2" t="s">
+      <c r="E41" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="H41" s="2" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>30</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>31</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>32</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>33</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>34</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J41" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="L41" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42">
+        <v>27</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="C42" s="2" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>131</v>
@@ -2300,18 +2502,27 @@
         <v>143</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="J42" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="L42" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43">
+        <v>28</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B43" s="3" t="s">
-        <v>44</v>
-      </c>
       <c r="C43" s="2" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>128</v>
@@ -2323,458 +2534,477 @@
         <v>143</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44">
+        <v>139</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="I43" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="J43" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="L43" t="s">
+        <v>159</v>
+      </c>
+      <c r="M43" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="J44" s="9" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="J45" s="9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="J46" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="J47" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="J48" s="9" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>29</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>38</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>39</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>40</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>41</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>42</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="C49" s="2" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>128</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G49" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H49" s="2"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>30</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="I50" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="J50" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="L50" t="s">
+        <v>159</v>
+      </c>
+      <c r="M50" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="J51" s="9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="J52" s="9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="J53" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>31</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>32</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="J55" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="L55" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>33</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="J56" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="L56" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="M56" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>34</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G57" s="2" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50">
+      <c r="H57" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="J57" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="L57" t="s">
+        <v>159</v>
+      </c>
+      <c r="M57" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>35</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51">
+      <c r="C58" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="I58" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="J58" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="L58" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="J59" s="9" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>36</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>45</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G52" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>46</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>47</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>48</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>49</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>50</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G57" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>51</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>52</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G59" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>53</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="C60" s="2" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>128</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G60" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>37</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G61" s="2" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>54</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G61" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H61" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="J61" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="L61" t="s">
+        <v>159</v>
+      </c>
+      <c r="M61" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>55</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>63</v>
+        <v>38</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>128</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>144</v>
@@ -2783,18 +3013,18 @@
         <v>145</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>57</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>65</v>
+        <v>40</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>128</v>
@@ -2806,21 +3036,21 @@
         <v>145</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>144</v>
@@ -2830,6 +3060,403 @@
       </c>
       <c r="G65" s="2" t="s">
         <v>137</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>42</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>43</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>44</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>45</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>46</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>47</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>48</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>49</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>50</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>51</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>52</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>53</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>54</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>55</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>56</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>57</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>58</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L85">
+        <f>COUNTIF(L2:L82, "Ja")</f>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>